<commit_message>
[optimize] add billitem_base cStyle 字段支持
</commit_message>
<xml_diff>
--- a/generate-sql/config/resource.xlsx
+++ b/generate-sql/config/resource.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30351" windowHeight="11451"/>
+    <workbookView windowHeight="22880"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="75">
   <si>
     <t>表名</t>
   </si>
@@ -233,6 +233,12 @@
   </si>
   <si>
     <t>操作日志操作按钮多语</t>
+  </si>
+  <si>
+    <t>cStyle</t>
+  </si>
+  <si>
+    <t>控件前端扩展使用字段</t>
   </si>
 </sst>
 </file>
@@ -240,10 +246,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -255,6 +261,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -262,7 +275,46 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -275,8 +327,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -290,26 +358,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -321,9 +374,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -337,11 +389,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -352,51 +403,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -419,187 +425,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -628,17 +634,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -654,6 +654,47 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -690,192 +731,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -892,59 +898,65 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="1" builtinId="52"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="2" builtinId="42"/>
+    <cellStyle name="强调文字颜色 4" xfId="3" builtinId="41"/>
+    <cellStyle name="输入" xfId="4" builtinId="20"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="5" builtinId="39"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="6" builtinId="38"/>
+    <cellStyle name="货币" xfId="7" builtinId="4"/>
+    <cellStyle name="强调文字颜色 3" xfId="8" builtinId="37"/>
+    <cellStyle name="百分比" xfId="9" builtinId="5"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="10" builtinId="36"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="11" builtinId="48"/>
+    <cellStyle name="强调文字颜色 2" xfId="12" builtinId="33"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="13" builtinId="32"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="14" builtinId="44"/>
+    <cellStyle name="计算" xfId="15" builtinId="22"/>
+    <cellStyle name="强调文字颜色 1" xfId="16" builtinId="29"/>
+    <cellStyle name="适中" xfId="17" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="18" builtinId="46"/>
+    <cellStyle name="好" xfId="19" builtinId="26"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="20" builtinId="30"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="差" xfId="22" builtinId="27"/>
+    <cellStyle name="检查单元格" xfId="23" builtinId="23"/>
     <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="标题 1" xfId="25" builtinId="16"/>
+    <cellStyle name="解释性文本" xfId="26" builtinId="53"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="27" builtinId="34"/>
+    <cellStyle name="标题 4" xfId="28" builtinId="19"/>
+    <cellStyle name="货币[0]" xfId="29" builtinId="7"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="30" builtinId="43"/>
+    <cellStyle name="千位分隔" xfId="31" builtinId="3"/>
+    <cellStyle name="已访问的超链接" xfId="32" builtinId="9"/>
+    <cellStyle name="标题" xfId="33" builtinId="15"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="34" builtinId="35"/>
+    <cellStyle name="警告文本" xfId="35" builtinId="11"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="注释" xfId="37" builtinId="10"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="38" builtinId="50"/>
+    <cellStyle name="强调文字颜色 5" xfId="39" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8"/>
+    <cellStyle name="千位分隔[0]" xfId="42" builtinId="6"/>
+    <cellStyle name="标题 2" xfId="43" builtinId="17"/>
     <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="标题 3" xfId="45" builtinId="18"/>
     <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="47" builtinId="31"/>
+    <cellStyle name="链接单元格" xfId="48" builtinId="24"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1213,22 +1225,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14414414414414" defaultRowHeight="14.1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="28.5585585585586" customWidth="1"/>
-    <col min="2" max="2" width="14.3423423423423" customWidth="1"/>
-    <col min="3" max="3" width="20.7117117117117" customWidth="1"/>
-    <col min="4" max="4" width="60.5855855855856" style="1" customWidth="1"/>
-    <col min="5" max="5" width="63.7117117117117" customWidth="1"/>
+    <col min="1" max="1" width="28.5625" customWidth="1"/>
+    <col min="2" max="2" width="14.3392857142857" customWidth="1"/>
+    <col min="3" max="3" width="20.7142857142857" customWidth="1"/>
+    <col min="4" max="4" width="60.5892857142857" style="1" customWidth="1"/>
+    <col min="5" max="5" width="63.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.15" spans="1:5">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1245,7 +1257,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="14.15" spans="1:5">
+    <row r="2" spans="1:5">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1262,7 +1274,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" ht="28.3" spans="1:5">
+    <row r="3" ht="24" spans="1:5">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -1279,7 +1291,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" ht="28.3" spans="1:5">
+    <row r="4" ht="24" spans="1:5">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -1296,7 +1308,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" ht="28.3" spans="1:5">
+    <row r="5" ht="24" spans="1:5">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
@@ -1313,7 +1325,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" ht="28.3" spans="1:5">
+    <row r="6" ht="24" spans="1:5">
       <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
@@ -1330,7 +1342,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" ht="28.3" spans="1:5">
+    <row r="7" ht="24" spans="1:5">
       <c r="A7" s="4" t="s">
         <v>20</v>
       </c>
@@ -1347,7 +1359,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" ht="28.3" spans="1:5">
+    <row r="8" ht="24" spans="1:5">
       <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
@@ -1364,7 +1376,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" ht="42.45" spans="1:5">
+    <row r="9" ht="36" spans="1:5">
       <c r="A9" s="4" t="s">
         <v>27</v>
       </c>
@@ -1381,7 +1393,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" ht="42.45" spans="1:5">
+    <row r="10" ht="36" spans="1:5">
       <c r="A10" s="4" t="s">
         <v>32</v>
       </c>
@@ -1398,7 +1410,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" ht="56.55" spans="1:5">
+    <row r="11" ht="48" spans="1:5">
       <c r="A11" s="4" t="s">
         <v>37</v>
       </c>
@@ -1415,7 +1427,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" ht="28.3" spans="1:5">
+    <row r="12" ht="24" spans="1:5">
       <c r="A12" s="4" t="s">
         <v>42</v>
       </c>
@@ -1587,6 +1599,23 @@
       </c>
       <c r="E23" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="24" ht="24" spans="1:5">
+      <c r="A24" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[optimize] support translation for cStyle(billtplgroup_base)
</commit_message>
<xml_diff>
--- a/generate-sql/config/resource.xlsx
+++ b/generate-sql/config/resource.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="75">
   <si>
     <t>表名</t>
   </si>
@@ -247,9 +247,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -261,13 +261,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -281,8 +274,91 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -305,7 +381,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -313,17 +389,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -334,75 +403,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -425,37 +425,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -467,7 +581,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -479,133 +599,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -637,23 +637,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -673,13 +658,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -708,15 +697,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -731,153 +711,173 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1225,10 +1225,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12" outlineLevelCol="4"/>
@@ -1618,6 +1618,17 @@
         <v>74</v>
       </c>
     </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>